<commit_message>
add class 1 traffic
</commit_message>
<xml_diff>
--- a/All Traffic Data_1996-2022_class1.xlsx
+++ b/All Traffic Data_1996-2022_class1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liuxi\Desktop\Research\2023.03.22 (FRA 2023)\Traffic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liuxi\Desktop\Research\2023.03.22 (FRA 2023)\Shiny plots\FRA_Visualizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A550C-6770-4839-9F0F-7A03EF49C08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73BBD85-FB14-46CE-A32F-CD8B39813CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="13866" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="9" r:id="rId1"/>
@@ -8735,7 +8735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3CF1C0-974A-4875-91CF-440ED9584AE4}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -11861,7 +11861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45722899-D95A-4A2F-A91F-3AF0C9F68B10}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>